<commit_message>
Add DTOs by Custom Queries
</commit_message>
<xml_diff>
--- a/Proyecto/Data/GenData.xlsx
+++ b/Proyecto/Data/GenData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Repositories\ServicesDevelopment\Proyecto\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F18F11-27B5-47C9-B142-8B6922B08BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC273511-468D-4EF3-93E1-085AD5E07BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{16BA8811-11E7-45E3-9022-F87FA0B716A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{16BA8811-11E7-45E3-9022-F87FA0B716A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -635,9 +635,6 @@
     <t>Tocar el Timbre</t>
   </si>
   <si>
-    <t>Pilas con el Perro que es Bravo</t>
-  </si>
-  <si>
     <t>Traer Vuelta de un billete de 50</t>
   </si>
   <si>
@@ -666,6 +663,9 @@
   </si>
   <si>
     <t>INSERT INTO `arepasdb`.`orderdetails` ( `OrderId`, `ProductId`, `Quantity`, `PriceOrd`) VALUES (</t>
+  </si>
+  <si>
+    <t>Estoy en casa de mi Novia</t>
   </si>
 </sst>
 </file>
@@ -3470,8 +3470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EBA7CE-4F47-4DBD-AE3C-ED34C3ED97FE}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3552,7 +3552,7 @@
         <v>197</v>
       </c>
       <c r="G2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H2">
         <f>A2</f>
@@ -3603,10 +3603,10 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -3618,21 +3618,21 @@
         <v>19000</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="G3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H6" si="0">A3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>190</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J6" si="1">B3</f>
-        <v>Sofia Herrera</v>
+        <f t="shared" ref="J3:J7" si="1">B3</f>
+        <v>Alejandro Gonzalez</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>152</v>
@@ -3659,15 +3659,15 @@
         <v>190</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" ref="R3:R6" si="5">F3</f>
-        <v>Pilas con el Perro que es Bravo</v>
+        <f t="shared" ref="R3:R5" si="5">F3</f>
+        <v>Estoy en casa de mi Novia</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>153</v>
       </c>
       <c r="U3" t="str">
         <f t="shared" ref="U3:U6" si="6">_xlfn.CONCAT(G3:S3)</f>
-        <v>INSERT INTO `arepasdb`.`orders` ( `CustomerId`, `DeliveryFullName`, `DeliveryAddress`, `DeliveryPhoneNumber`, `TotalPrice`, `Notes`) VALUES (2,'Sofia Herrera','Avenida 3N # 8-56, Barrio Granada','311-234-5678',19000,'Pilas con el Perro que es Bravo');</v>
+        <v>INSERT INTO `arepasdb`.`orders` ( `CustomerId`, `DeliveryFullName`, `DeliveryAddress`, `DeliveryPhoneNumber`, `TotalPrice`, `Notes`) VALUES (1,'Alejandro Gonzalez','Avenida 3N # 8-56, Barrio Granada','311-234-5678',19000,'Estoy en casa de mi Novia');</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -3687,10 +3687,10 @@
         <v>26000</v>
       </c>
       <c r="F4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
@@ -3756,10 +3756,10 @@
         <v>18000</v>
       </c>
       <c r="F5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
@@ -3825,7 +3825,7 @@
         <v>12000</v>
       </c>
       <c r="G6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
@@ -3860,13 +3860,13 @@
         <v>12000</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R6" t="s">
         <v>158</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" si="6"/>
@@ -3882,7 +3882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E6FB85-4EC2-426E-8E3D-5BC28FDA42F6}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -3899,29 +3899,29 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" t="s">
         <v>201</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>202</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>203</v>
       </c>
-      <c r="D1" t="s">
-        <v>204</v>
-      </c>
       <c r="F1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J1" t="s">
         <v>202</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>203</v>
-      </c>
-      <c r="L1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -3938,35 +3938,35 @@
         <v>2500</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F2">
         <f>A2</f>
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H2">
         <f>B2</f>
         <v>2</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J2">
         <f>C2</f>
         <v>1</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L2">
         <f>D2</f>
         <v>2500</v>
       </c>
       <c r="M2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O2" t="str">
         <f>_xlfn.CONCAT(E2:M2)</f>
@@ -3987,35 +3987,35 @@
         <v>3000</v>
       </c>
       <c r="E3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F11" si="0">A3</f>
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H11" si="1">B3</f>
         <v>4</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J11" si="2">C3</f>
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L11" si="3">D3</f>
         <v>3000</v>
       </c>
       <c r="M3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" ref="O3:O11" si="4">_xlfn.CONCAT(E3:M3)</f>
@@ -4036,35 +4036,35 @@
         <v>12000</v>
       </c>
       <c r="E4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L4">
         <f t="shared" si="3"/>
         <v>12000</v>
       </c>
       <c r="M4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="4"/>
@@ -4085,35 +4085,35 @@
         <v>7000</v>
       </c>
       <c r="E5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L5">
         <f t="shared" si="3"/>
         <v>7000</v>
       </c>
       <c r="M5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="4"/>
@@ -4134,35 +4134,35 @@
         <v>26000</v>
       </c>
       <c r="E6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L6">
         <f t="shared" si="3"/>
         <v>26000</v>
       </c>
       <c r="M6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="4"/>
@@ -4183,35 +4183,35 @@
         <v>5000</v>
       </c>
       <c r="E7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L7">
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="M7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="4"/>
@@ -4232,35 +4232,35 @@
         <v>6000</v>
       </c>
       <c r="E8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
         <v>6000</v>
       </c>
       <c r="M8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="4"/>
@@ -4281,35 +4281,35 @@
         <v>7000</v>
       </c>
       <c r="E9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
         <v>7000</v>
       </c>
       <c r="M9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="4"/>
@@ -4330,35 +4330,35 @@
         <v>4000</v>
       </c>
       <c r="E10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
         <v>4000</v>
       </c>
       <c r="M10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="4"/>
@@ -4379,35 +4379,35 @@
         <v>8000</v>
       </c>
       <c r="E11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
         <v>8000</v>
       </c>
       <c r="M11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="4"/>

</xml_diff>